<commit_message>
implementatie van controllers, repositories en services voor het correct inloggen. Nog te testen cuz of DB...
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t xml:space="preserve">Naam student 1:</t>
   </si>
@@ -49,7 +49,13 @@
     <t xml:space="preserve">Basisconfiguratie model (klassen aanmaken, methodes aanmaken, attributen aanmaken…)</t>
   </si>
   <si>
-    <t xml:space="preserve">basisnavigatie main controller</t>
+    <t xml:space="preserve">Basisnavigatie main controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementatie van Repositories, services en controllers zodat personen kunnen inloggen op de correcte manier (nog te testen, want connectie met DB doet moeilijk)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/12/2024</t>
   </si>
 </sst>
 </file>
@@ -161,44 +167,56 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -455,377 +473,385 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="5" t="n">
         <v>45424</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="6" t="n">
         <v>0.5</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>45547</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="5" t="n">
         <v>45547</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="6" t="n">
         <v>0.5</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+    <row r="7" customFormat="false" ht="116.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="8"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="8"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="8"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="8"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="8"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="8"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="8"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="8"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D55" s="9"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D56" s="9"/>
+      <c r="D56" s="12"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D57" s="9"/>
+      <c r="D57" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
mijn changes van de dag :)
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t xml:space="preserve">Naam student 1:</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Basisnavigatie main controller</t>
   </si>
   <si>
-    <t xml:space="preserve">Implementatie van Repositories, services en controllers zodat personen kunnen inloggen op de correcte manier (nog te testen, want connectie met DB doet moeilijk)</t>
+    <t xml:space="preserve">Implementatie van Repositories, services en controllers zodat personen kunnen inloggen op de correcte manier (nog te testen, want connectie met DB bestaat nog niet)</t>
   </si>
   <si>
     <t xml:space="preserve">15/12/2024</t>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Heraanpassen van het model zoadt dit overeenkomt met de databank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creeeren van index pagina voor de klant. Deze kan nu al de beschreven acties doen.</t>
   </si>
 </sst>
 </file>
@@ -494,14 +497,14 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.5"/>
   </cols>
   <sheetData>
@@ -595,7 +598,7 @@
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="6" t="n">
@@ -609,7 +612,7 @@
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="6" t="n">
@@ -623,7 +626,7 @@
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="6" t="n">
@@ -637,7 +640,7 @@
       <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="6" t="n">
@@ -647,11 +650,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+    <row r="12" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>

</xml_diff>

<commit_message>
verbeteringen peoplecontroller (afstelling db)
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t xml:space="preserve">Naam student 1:</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t xml:space="preserve">25/12/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debuggen van de PeopleController (afstellen met nieuwe back-end en db)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/12/2024</t>
   </si>
 </sst>
 </file>
@@ -502,8 +508,8 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,11 +690,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+    <row r="14" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7"/>
@@ -809,11 +823,11 @@
       <c r="B34" s="11"/>
       <c r="C34" s="12" t="n">
         <f aca="false">SUM(C4:C33)</f>
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
       <c r="D34" s="12" t="n">
         <f aca="false">SUM(D4:D33)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>